<commit_message>
#138-Introduced more information on Sales per customer and Ending Inventory report
</commit_message>
<xml_diff>
--- a/Beelina.API/Templates/ReportTemplates/EndingInventoryPerProductReport_Template.xlsx
+++ b/Beelina.API/Templates/ReportTemplates/EndingInventoryPerProductReport_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Beelina\Beelina.API\Templates\ReportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B5A02D-522E-4767-BBCE-AFC9979D4E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AA183C-9E57-4F70-A5E3-E74FA4A22F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4BCE0149-8C23-4351-A0DE-0EABB1405EDD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Item Code</t>
   </si>
@@ -54,6 +54,21 @@
   </si>
   <si>
     <t>Ending Stocks Value</t>
+  </si>
+  <si>
+    <t>Sales Agent Name:</t>
+  </si>
+  <si>
+    <t>From Date:</t>
+  </si>
+  <si>
+    <t>To Date:</t>
+  </si>
+  <si>
+    <t>Sold Stocks</t>
+  </si>
+  <si>
+    <t>Sold Stocks Value</t>
   </si>
 </sst>
 </file>
@@ -97,7 +112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -106,6 +121,10 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FECBADA-66F2-4187-ACE2-9435ED0DBF8B}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,26 +452,57 @@
     <col min="4" max="4" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1"/>
+      <c r="F1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="D2"/>
+      <c r="F2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="D3"/>
+      <c r="F3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>